<commit_message>
Working On Nav Bar
</commit_message>
<xml_diff>
--- a/2025 Track.xlsx
+++ b/2025 Track.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\my-hub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2CB4B9A-B9B4-4340-8CCD-345DDFD347B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAD5DDE7-F0BA-4F8E-B93B-4540277C2639}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Today" sheetId="10" r:id="rId1"/>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="33">
   <si>
     <t>Date</t>
   </si>
@@ -728,9 +728,6 @@
     <xf numFmtId="1" fontId="4" fillId="3" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -766,6 +763,9 @@
     </xf>
     <xf numFmtId="14" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1948,8 +1948,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEAD7C17-09EB-4F73-A124-CCFB578ED3D8}">
   <dimension ref="B1:E369"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1961,10 +1961,12 @@
   <sheetData>
     <row r="1" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="45" t="s">
+      <c r="B2" s="57" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="45"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
     </row>
     <row r="3" spans="2:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="33" t="s">
@@ -3605,7 +3607,7 @@
       </c>
       <c r="D99" s="36" t="str">
         <f>IF('2025'!$K100="DONE","Done","")</f>
-        <v/>
+        <v>Done</v>
       </c>
       <c r="E99" s="36" t="str">
         <f>IF('2025'!$Q100="DONE","Done","")</f>
@@ -3622,7 +3624,7 @@
       </c>
       <c r="D100" s="36" t="str">
         <f>IF('2025'!$K101="DONE","Done","")</f>
-        <v/>
+        <v>Done</v>
       </c>
       <c r="E100" s="36" t="str">
         <f>IF('2025'!$Q101="DONE","Done","")</f>
@@ -8188,7 +8190,7 @@
     <row r="369" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B2:E2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8198,8 +8200,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DCCB1A6-4234-460B-9354-2A4319EE0C90}">
   <dimension ref="A1:R371"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="P6" sqref="P6"/>
+    <sheetView topLeftCell="F94" workbookViewId="0">
+      <selection activeCell="K101" sqref="K101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -8219,70 +8221,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="124.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="48" t="s">
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
-      <c r="L1" s="46"/>
-      <c r="M1" s="46"/>
-      <c r="N1" s="48" t="s">
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
+      <c r="K1" s="45"/>
+      <c r="L1" s="45"/>
+      <c r="M1" s="45"/>
+      <c r="N1" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="O1" s="46"/>
-      <c r="P1" s="46"/>
-      <c r="Q1" s="46"/>
-      <c r="R1" s="46"/>
+      <c r="O1" s="45"/>
+      <c r="P1" s="45"/>
+      <c r="Q1" s="45"/>
+      <c r="R1" s="45"/>
     </row>
     <row r="2" spans="1:18" ht="21.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="47" t="s">
+      <c r="B2" s="46" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
       <c r="F2" s="3" t="s">
         <v>4</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="49" t="s">
+      <c r="H2" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="I2" s="47"/>
-      <c r="J2" s="47"/>
-      <c r="K2" s="47"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="46"/>
+      <c r="K2" s="46"/>
       <c r="L2" s="3" t="s">
         <v>4</v>
       </c>
       <c r="M2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="N2" s="49" t="s">
+      <c r="N2" s="48" t="s">
         <v>30</v>
       </c>
-      <c r="O2" s="47"/>
-      <c r="P2" s="47"/>
-      <c r="Q2" s="47"/>
-      <c r="R2" s="52" t="s">
+      <c r="O2" s="46"/>
+      <c r="P2" s="46"/>
+      <c r="Q2" s="46"/>
+      <c r="R2" s="51" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:18" ht="21.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="47"/>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
+      <c r="B3" s="46"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
       <c r="F3" s="26">
         <f>(F4/60)+(G4/3600)</f>
         <v>3.1205555555555557</v>
@@ -8291,23 +8293,23 @@
         <f>F4+(G4/60)</f>
         <v>187.23333333333335</v>
       </c>
-      <c r="H3" s="50"/>
-      <c r="I3" s="51"/>
-      <c r="J3" s="51"/>
-      <c r="K3" s="51"/>
+      <c r="H3" s="49"/>
+      <c r="I3" s="50"/>
+      <c r="J3" s="50"/>
+      <c r="K3" s="50"/>
       <c r="L3" s="26">
         <f>(L4/60)+(M4/3600)</f>
-        <v>1.1138888888888889</v>
+        <v>1.2616666666666667</v>
       </c>
       <c r="M3" s="25">
         <f>L4+(M4/60)</f>
-        <v>66.833333333333329</v>
-      </c>
-      <c r="N3" s="50"/>
-      <c r="O3" s="51"/>
-      <c r="P3" s="51"/>
-      <c r="Q3" s="51"/>
-      <c r="R3" s="53"/>
+        <v>75.7</v>
+      </c>
+      <c r="N3" s="49"/>
+      <c r="O3" s="50"/>
+      <c r="P3" s="50"/>
+      <c r="Q3" s="50"/>
+      <c r="R3" s="52"/>
     </row>
     <row r="4" spans="1:18" ht="21.6" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A4" s="24" t="s">
@@ -8347,11 +8349,11 @@
       </c>
       <c r="L4" s="7">
         <f>SUMIFS(L$5:L$369,$K$5:$K$369,"DONE")</f>
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="M4" s="7">
         <f>SUMIFS(M$5:M$369,$K$5:$K$369,"DONE")</f>
-        <v>590</v>
+        <v>702</v>
       </c>
       <c r="N4" s="39" t="s">
         <v>0</v>
@@ -13230,9 +13232,11 @@
       </c>
       <c r="J100" s="1">
         <f t="shared" si="10"/>
-        <v>4.5937499999999985E-2</v>
-      </c>
-      <c r="K100" s="28"/>
+        <v>4.9328703703703687E-2</v>
+      </c>
+      <c r="K100" s="28" t="s">
+        <v>6</v>
+      </c>
       <c r="L100" s="2">
         <v>4</v>
       </c>
@@ -13276,13 +13280,15 @@
       </c>
       <c r="I101" s="1">
         <f t="shared" si="9"/>
-        <v>4.5937499999999985E-2</v>
+        <v>4.9328703703703687E-2</v>
       </c>
       <c r="J101" s="1">
         <f t="shared" si="10"/>
-        <v>4.5937499999999985E-2</v>
-      </c>
-      <c r="K101" s="28"/>
+        <v>5.2094907407407388E-2</v>
+      </c>
+      <c r="K101" s="28" t="s">
+        <v>6</v>
+      </c>
       <c r="L101" s="2">
         <v>3</v>
       </c>
@@ -13326,11 +13332,11 @@
       </c>
       <c r="I102" s="1">
         <f t="shared" si="9"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J102" s="1">
         <f t="shared" si="10"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K102" s="28"/>
       <c r="L102" s="2"/>
@@ -13372,11 +13378,11 @@
       </c>
       <c r="I103" s="1">
         <f t="shared" si="9"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J103" s="1">
         <f t="shared" si="10"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K103" s="28"/>
       <c r="L103" s="2"/>
@@ -13418,11 +13424,11 @@
       </c>
       <c r="I104" s="1">
         <f t="shared" si="9"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J104" s="1">
         <f t="shared" si="10"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K104" s="28"/>
       <c r="L104" s="2"/>
@@ -13464,11 +13470,11 @@
       </c>
       <c r="I105" s="1">
         <f t="shared" si="9"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J105" s="1">
         <f t="shared" si="10"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K105" s="28"/>
       <c r="L105" s="2"/>
@@ -13510,11 +13516,11 @@
       </c>
       <c r="I106" s="1">
         <f t="shared" si="9"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J106" s="1">
         <f t="shared" si="10"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K106" s="28"/>
       <c r="L106" s="2"/>
@@ -13556,11 +13562,11 @@
       </c>
       <c r="I107" s="1">
         <f t="shared" si="9"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J107" s="1">
         <f t="shared" si="10"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K107" s="28"/>
       <c r="L107" s="2"/>
@@ -13602,11 +13608,11 @@
       </c>
       <c r="I108" s="1">
         <f t="shared" si="9"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J108" s="1">
         <f t="shared" si="10"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K108" s="28"/>
       <c r="L108" s="2"/>
@@ -13648,11 +13654,11 @@
       </c>
       <c r="I109" s="1">
         <f t="shared" si="9"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J109" s="1">
         <f t="shared" si="10"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K109" s="28"/>
       <c r="L109" s="2"/>
@@ -13694,11 +13700,11 @@
       </c>
       <c r="I110" s="1">
         <f t="shared" si="9"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J110" s="1">
         <f t="shared" si="10"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K110" s="28"/>
       <c r="L110" s="2"/>
@@ -13740,11 +13746,11 @@
       </c>
       <c r="I111" s="1">
         <f t="shared" si="9"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J111" s="1">
         <f t="shared" si="10"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K111" s="28"/>
       <c r="L111" s="2"/>
@@ -13786,11 +13792,11 @@
       </c>
       <c r="I112" s="1">
         <f t="shared" si="9"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J112" s="1">
         <f t="shared" si="10"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K112" s="28"/>
       <c r="L112" s="2"/>
@@ -13832,11 +13838,11 @@
       </c>
       <c r="I113" s="1">
         <f t="shared" si="9"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J113" s="1">
         <f t="shared" si="10"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K113" s="28"/>
       <c r="L113" s="2"/>
@@ -13878,11 +13884,11 @@
       </c>
       <c r="I114" s="1">
         <f t="shared" si="9"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J114" s="1">
         <f t="shared" si="10"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K114" s="28"/>
       <c r="L114" s="2"/>
@@ -13924,11 +13930,11 @@
       </c>
       <c r="I115" s="1">
         <f t="shared" si="9"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J115" s="1">
         <f t="shared" si="10"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K115" s="28"/>
       <c r="L115" s="2"/>
@@ -13970,11 +13976,11 @@
       </c>
       <c r="I116" s="1">
         <f t="shared" si="9"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J116" s="1">
         <f t="shared" si="10"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K116" s="28"/>
       <c r="L116" s="2"/>
@@ -14016,11 +14022,11 @@
       </c>
       <c r="I117" s="1">
         <f t="shared" si="9"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J117" s="1">
         <f t="shared" si="10"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K117" s="28"/>
       <c r="L117" s="2"/>
@@ -14062,11 +14068,11 @@
       </c>
       <c r="I118" s="1">
         <f t="shared" si="9"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J118" s="1">
         <f t="shared" si="10"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K118" s="28"/>
       <c r="L118" s="2"/>
@@ -14108,11 +14114,11 @@
       </c>
       <c r="I119" s="1">
         <f t="shared" si="9"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J119" s="1">
         <f t="shared" si="10"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K119" s="28"/>
       <c r="L119" s="2"/>
@@ -14154,11 +14160,11 @@
       </c>
       <c r="I120" s="1">
         <f t="shared" si="9"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J120" s="1">
         <f t="shared" si="10"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K120" s="28"/>
       <c r="L120" s="2"/>
@@ -14200,11 +14206,11 @@
       </c>
       <c r="I121" s="1">
         <f t="shared" si="9"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J121" s="1">
         <f t="shared" si="10"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K121" s="28"/>
       <c r="L121" s="2"/>
@@ -14246,11 +14252,11 @@
       </c>
       <c r="I122" s="1">
         <f t="shared" si="9"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J122" s="1">
         <f t="shared" si="10"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K122" s="28"/>
       <c r="L122" s="2"/>
@@ -14292,11 +14298,11 @@
       </c>
       <c r="I123" s="1">
         <f t="shared" si="9"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J123" s="1">
         <f t="shared" si="10"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K123" s="28"/>
       <c r="L123" s="2"/>
@@ -14338,11 +14344,11 @@
       </c>
       <c r="I124" s="1">
         <f t="shared" si="9"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J124" s="1">
         <f t="shared" si="10"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K124" s="28"/>
       <c r="L124" s="2"/>
@@ -14384,11 +14390,11 @@
       </c>
       <c r="I125" s="1">
         <f t="shared" si="9"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J125" s="1">
         <f t="shared" si="10"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K125" s="28"/>
       <c r="L125" s="2"/>
@@ -14430,11 +14436,11 @@
       </c>
       <c r="I126" s="1">
         <f t="shared" si="9"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J126" s="1">
         <f t="shared" si="10"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K126" s="28"/>
       <c r="L126" s="2"/>
@@ -14476,11 +14482,11 @@
       </c>
       <c r="I127" s="1">
         <f t="shared" si="9"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J127" s="1">
         <f t="shared" si="10"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K127" s="28"/>
       <c r="L127" s="2"/>
@@ -14522,11 +14528,11 @@
       </c>
       <c r="I128" s="1">
         <f t="shared" si="9"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J128" s="1">
         <f t="shared" si="10"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K128" s="28"/>
       <c r="L128" s="2"/>
@@ -14568,11 +14574,11 @@
       </c>
       <c r="I129" s="1">
         <f t="shared" si="9"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J129" s="1">
         <f t="shared" si="10"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K129" s="28"/>
       <c r="L129" s="2"/>
@@ -14614,11 +14620,11 @@
       </c>
       <c r="I130" s="1">
         <f t="shared" si="9"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J130" s="1">
         <f t="shared" si="10"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K130" s="28"/>
       <c r="L130" s="2"/>
@@ -14660,11 +14666,11 @@
       </c>
       <c r="I131" s="1">
         <f t="shared" si="9"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J131" s="1">
         <f t="shared" si="10"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K131" s="28"/>
       <c r="L131" s="2"/>
@@ -14706,11 +14712,11 @@
       </c>
       <c r="I132" s="1">
         <f t="shared" si="9"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J132" s="1">
         <f t="shared" si="10"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K132" s="28"/>
       <c r="L132" s="2"/>
@@ -14752,11 +14758,11 @@
       </c>
       <c r="I133" s="1">
         <f t="shared" si="9"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J133" s="1">
         <f t="shared" si="10"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K133" s="28"/>
       <c r="L133" s="2"/>
@@ -14798,11 +14804,11 @@
       </c>
       <c r="I134" s="1">
         <f t="shared" si="9"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J134" s="1">
         <f t="shared" si="10"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K134" s="28"/>
       <c r="L134" s="2"/>
@@ -14844,11 +14850,11 @@
       </c>
       <c r="I135" s="1">
         <f t="shared" ref="I135:I198" si="15">J134</f>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J135" s="1">
         <f t="shared" ref="J135:J198" si="16">IF(K135="DONE",I135+(L135/1440)+(M135/86400),I135)</f>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K135" s="28"/>
       <c r="L135" s="2"/>
@@ -14890,11 +14896,11 @@
       </c>
       <c r="I136" s="1">
         <f t="shared" si="15"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J136" s="1">
         <f t="shared" si="16"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K136" s="28"/>
       <c r="L136" s="2"/>
@@ -14936,11 +14942,11 @@
       </c>
       <c r="I137" s="1">
         <f t="shared" si="15"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J137" s="1">
         <f t="shared" si="16"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K137" s="28"/>
       <c r="L137" s="2"/>
@@ -14982,11 +14988,11 @@
       </c>
       <c r="I138" s="1">
         <f t="shared" si="15"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J138" s="1">
         <f t="shared" si="16"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K138" s="28"/>
       <c r="L138" s="2"/>
@@ -15028,11 +15034,11 @@
       </c>
       <c r="I139" s="1">
         <f t="shared" si="15"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J139" s="1">
         <f t="shared" si="16"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K139" s="28"/>
       <c r="L139" s="2"/>
@@ -15074,11 +15080,11 @@
       </c>
       <c r="I140" s="1">
         <f t="shared" si="15"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J140" s="1">
         <f t="shared" si="16"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K140" s="28"/>
       <c r="L140" s="2"/>
@@ -15120,11 +15126,11 @@
       </c>
       <c r="I141" s="1">
         <f t="shared" si="15"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J141" s="1">
         <f t="shared" si="16"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K141" s="28"/>
       <c r="L141" s="2"/>
@@ -15166,11 +15172,11 @@
       </c>
       <c r="I142" s="1">
         <f t="shared" si="15"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J142" s="1">
         <f t="shared" si="16"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K142" s="28"/>
       <c r="L142" s="2"/>
@@ -15212,11 +15218,11 @@
       </c>
       <c r="I143" s="1">
         <f t="shared" si="15"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J143" s="1">
         <f t="shared" si="16"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K143" s="28"/>
       <c r="L143" s="2"/>
@@ -15258,11 +15264,11 @@
       </c>
       <c r="I144" s="1">
         <f t="shared" si="15"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J144" s="1">
         <f t="shared" si="16"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K144" s="28"/>
       <c r="L144" s="2"/>
@@ -15304,11 +15310,11 @@
       </c>
       <c r="I145" s="1">
         <f t="shared" si="15"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J145" s="1">
         <f t="shared" si="16"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K145" s="28"/>
       <c r="L145" s="2"/>
@@ -15350,11 +15356,11 @@
       </c>
       <c r="I146" s="1">
         <f t="shared" si="15"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J146" s="1">
         <f t="shared" si="16"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K146" s="28"/>
       <c r="L146" s="2"/>
@@ -15396,11 +15402,11 @@
       </c>
       <c r="I147" s="1">
         <f t="shared" si="15"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J147" s="1">
         <f t="shared" si="16"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K147" s="28"/>
       <c r="L147" s="2"/>
@@ -15442,11 +15448,11 @@
       </c>
       <c r="I148" s="1">
         <f t="shared" si="15"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J148" s="1">
         <f t="shared" si="16"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K148" s="28"/>
       <c r="L148" s="2"/>
@@ -15488,11 +15494,11 @@
       </c>
       <c r="I149" s="1">
         <f t="shared" si="15"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J149" s="1">
         <f t="shared" si="16"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K149" s="28"/>
       <c r="L149" s="2"/>
@@ -15534,11 +15540,11 @@
       </c>
       <c r="I150" s="1">
         <f t="shared" si="15"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J150" s="1">
         <f t="shared" si="16"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K150" s="28"/>
       <c r="L150" s="2"/>
@@ -15580,11 +15586,11 @@
       </c>
       <c r="I151" s="1">
         <f t="shared" si="15"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J151" s="1">
         <f t="shared" si="16"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K151" s="28"/>
       <c r="L151" s="2"/>
@@ -15626,11 +15632,11 @@
       </c>
       <c r="I152" s="1">
         <f t="shared" si="15"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J152" s="1">
         <f t="shared" si="16"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K152" s="28"/>
       <c r="L152" s="2"/>
@@ -15672,11 +15678,11 @@
       </c>
       <c r="I153" s="1">
         <f t="shared" si="15"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J153" s="1">
         <f t="shared" si="16"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K153" s="28"/>
       <c r="L153" s="2"/>
@@ -15718,11 +15724,11 @@
       </c>
       <c r="I154" s="1">
         <f t="shared" si="15"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J154" s="1">
         <f t="shared" si="16"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K154" s="28"/>
       <c r="L154" s="2"/>
@@ -15764,11 +15770,11 @@
       </c>
       <c r="I155" s="1">
         <f t="shared" si="15"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J155" s="1">
         <f t="shared" si="16"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K155" s="28"/>
       <c r="L155" s="2"/>
@@ -15810,11 +15816,11 @@
       </c>
       <c r="I156" s="1">
         <f t="shared" si="15"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J156" s="1">
         <f t="shared" si="16"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K156" s="28"/>
       <c r="L156" s="2"/>
@@ -15856,11 +15862,11 @@
       </c>
       <c r="I157" s="1">
         <f t="shared" si="15"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J157" s="1">
         <f t="shared" si="16"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K157" s="28"/>
       <c r="L157" s="2"/>
@@ -15902,11 +15908,11 @@
       </c>
       <c r="I158" s="1">
         <f t="shared" si="15"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J158" s="1">
         <f t="shared" si="16"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K158" s="28"/>
       <c r="L158" s="2"/>
@@ -15948,11 +15954,11 @@
       </c>
       <c r="I159" s="1">
         <f t="shared" si="15"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J159" s="1">
         <f t="shared" si="16"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K159" s="28"/>
       <c r="L159" s="2"/>
@@ -15994,11 +16000,11 @@
       </c>
       <c r="I160" s="1">
         <f t="shared" si="15"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J160" s="1">
         <f t="shared" si="16"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K160" s="28"/>
       <c r="L160" s="2"/>
@@ -16040,11 +16046,11 @@
       </c>
       <c r="I161" s="1">
         <f t="shared" si="15"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J161" s="1">
         <f t="shared" si="16"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K161" s="28"/>
       <c r="L161" s="2"/>
@@ -16086,11 +16092,11 @@
       </c>
       <c r="I162" s="1">
         <f t="shared" si="15"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J162" s="1">
         <f t="shared" si="16"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K162" s="28"/>
       <c r="L162" s="2"/>
@@ -16132,11 +16138,11 @@
       </c>
       <c r="I163" s="1">
         <f t="shared" si="15"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J163" s="1">
         <f t="shared" si="16"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K163" s="28"/>
       <c r="L163" s="2"/>
@@ -16178,11 +16184,11 @@
       </c>
       <c r="I164" s="1">
         <f t="shared" si="15"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J164" s="1">
         <f t="shared" si="16"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K164" s="28"/>
       <c r="L164" s="2"/>
@@ -16224,11 +16230,11 @@
       </c>
       <c r="I165" s="1">
         <f t="shared" si="15"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J165" s="1">
         <f t="shared" si="16"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K165" s="28"/>
       <c r="L165" s="2"/>
@@ -16270,11 +16276,11 @@
       </c>
       <c r="I166" s="1">
         <f t="shared" si="15"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J166" s="1">
         <f t="shared" si="16"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K166" s="28"/>
       <c r="L166" s="2"/>
@@ -16316,11 +16322,11 @@
       </c>
       <c r="I167" s="1">
         <f t="shared" si="15"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J167" s="1">
         <f t="shared" si="16"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K167" s="28"/>
       <c r="L167" s="2"/>
@@ -16362,11 +16368,11 @@
       </c>
       <c r="I168" s="1">
         <f t="shared" si="15"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J168" s="1">
         <f t="shared" si="16"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K168" s="28"/>
       <c r="L168" s="2"/>
@@ -16408,11 +16414,11 @@
       </c>
       <c r="I169" s="1">
         <f t="shared" si="15"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J169" s="1">
         <f t="shared" si="16"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K169" s="28"/>
       <c r="L169" s="2"/>
@@ -16454,11 +16460,11 @@
       </c>
       <c r="I170" s="1">
         <f t="shared" si="15"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J170" s="1">
         <f t="shared" si="16"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K170" s="28"/>
       <c r="L170" s="2"/>
@@ -16500,11 +16506,11 @@
       </c>
       <c r="I171" s="1">
         <f t="shared" si="15"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J171" s="1">
         <f t="shared" si="16"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K171" s="28"/>
       <c r="L171" s="2"/>
@@ -16546,11 +16552,11 @@
       </c>
       <c r="I172" s="1">
         <f t="shared" si="15"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J172" s="1">
         <f t="shared" si="16"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K172" s="28"/>
       <c r="L172" s="2"/>
@@ -16592,11 +16598,11 @@
       </c>
       <c r="I173" s="1">
         <f t="shared" si="15"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J173" s="1">
         <f t="shared" si="16"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K173" s="28"/>
       <c r="L173" s="2"/>
@@ -16638,11 +16644,11 @@
       </c>
       <c r="I174" s="1">
         <f t="shared" si="15"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J174" s="1">
         <f t="shared" si="16"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K174" s="28"/>
       <c r="L174" s="2"/>
@@ -16684,11 +16690,11 @@
       </c>
       <c r="I175" s="1">
         <f t="shared" si="15"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J175" s="1">
         <f t="shared" si="16"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K175" s="28"/>
       <c r="L175" s="2"/>
@@ -16730,11 +16736,11 @@
       </c>
       <c r="I176" s="1">
         <f t="shared" si="15"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J176" s="1">
         <f t="shared" si="16"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K176" s="28"/>
       <c r="L176" s="2"/>
@@ -16776,11 +16782,11 @@
       </c>
       <c r="I177" s="1">
         <f t="shared" si="15"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J177" s="1">
         <f t="shared" si="16"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K177" s="28"/>
       <c r="L177" s="2"/>
@@ -16822,11 +16828,11 @@
       </c>
       <c r="I178" s="1">
         <f t="shared" si="15"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J178" s="1">
         <f t="shared" si="16"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K178" s="28"/>
       <c r="L178" s="2"/>
@@ -16868,11 +16874,11 @@
       </c>
       <c r="I179" s="1">
         <f t="shared" si="15"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J179" s="1">
         <f t="shared" si="16"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K179" s="28"/>
       <c r="L179" s="2"/>
@@ -16914,11 +16920,11 @@
       </c>
       <c r="I180" s="1">
         <f t="shared" si="15"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J180" s="1">
         <f t="shared" si="16"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K180" s="28"/>
       <c r="L180" s="2"/>
@@ -16960,11 +16966,11 @@
       </c>
       <c r="I181" s="1">
         <f t="shared" si="15"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J181" s="1">
         <f t="shared" si="16"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K181" s="28"/>
       <c r="L181" s="2"/>
@@ -17006,11 +17012,11 @@
       </c>
       <c r="I182" s="1">
         <f t="shared" si="15"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J182" s="1">
         <f t="shared" si="16"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K182" s="28"/>
       <c r="L182" s="2"/>
@@ -17052,11 +17058,11 @@
       </c>
       <c r="I183" s="1">
         <f t="shared" si="15"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J183" s="1">
         <f t="shared" si="16"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K183" s="28"/>
       <c r="L183" s="2"/>
@@ -17098,11 +17104,11 @@
       </c>
       <c r="I184" s="1">
         <f t="shared" si="15"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J184" s="1">
         <f t="shared" si="16"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K184" s="28"/>
       <c r="L184" s="2"/>
@@ -17144,11 +17150,11 @@
       </c>
       <c r="I185" s="1">
         <f t="shared" si="15"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J185" s="1">
         <f t="shared" si="16"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K185" s="28"/>
       <c r="L185" s="2"/>
@@ -17190,11 +17196,11 @@
       </c>
       <c r="I186" s="1">
         <f t="shared" si="15"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J186" s="1">
         <f t="shared" si="16"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K186" s="28"/>
       <c r="L186" s="2"/>
@@ -17236,11 +17242,11 @@
       </c>
       <c r="I187" s="1">
         <f t="shared" si="15"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J187" s="1">
         <f t="shared" si="16"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K187" s="28"/>
       <c r="L187" s="2"/>
@@ -17282,11 +17288,11 @@
       </c>
       <c r="I188" s="1">
         <f t="shared" si="15"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J188" s="1">
         <f t="shared" si="16"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K188" s="28"/>
       <c r="L188" s="2"/>
@@ -17328,11 +17334,11 @@
       </c>
       <c r="I189" s="1">
         <f t="shared" si="15"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J189" s="1">
         <f t="shared" si="16"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K189" s="28"/>
       <c r="L189" s="2"/>
@@ -17374,11 +17380,11 @@
       </c>
       <c r="I190" s="1">
         <f t="shared" si="15"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J190" s="1">
         <f t="shared" si="16"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K190" s="28"/>
       <c r="L190" s="2"/>
@@ -17420,11 +17426,11 @@
       </c>
       <c r="I191" s="1">
         <f t="shared" si="15"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J191" s="1">
         <f t="shared" si="16"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K191" s="28"/>
       <c r="L191" s="2"/>
@@ -17466,11 +17472,11 @@
       </c>
       <c r="I192" s="1">
         <f t="shared" si="15"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J192" s="1">
         <f t="shared" si="16"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K192" s="28"/>
       <c r="L192" s="2"/>
@@ -17512,11 +17518,11 @@
       </c>
       <c r="I193" s="1">
         <f t="shared" si="15"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J193" s="1">
         <f t="shared" si="16"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K193" s="28"/>
       <c r="L193" s="2"/>
@@ -17558,11 +17564,11 @@
       </c>
       <c r="I194" s="1">
         <f t="shared" si="15"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J194" s="1">
         <f t="shared" si="16"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K194" s="28"/>
       <c r="L194" s="2"/>
@@ -17604,11 +17610,11 @@
       </c>
       <c r="I195" s="1">
         <f t="shared" si="15"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J195" s="1">
         <f t="shared" si="16"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K195" s="28"/>
       <c r="L195" s="2"/>
@@ -17650,11 +17656,11 @@
       </c>
       <c r="I196" s="1">
         <f t="shared" si="15"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J196" s="1">
         <f t="shared" si="16"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K196" s="28"/>
       <c r="L196" s="2"/>
@@ -17696,11 +17702,11 @@
       </c>
       <c r="I197" s="1">
         <f t="shared" si="15"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J197" s="1">
         <f t="shared" si="16"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K197" s="28"/>
       <c r="L197" s="2"/>
@@ -17742,11 +17748,11 @@
       </c>
       <c r="I198" s="1">
         <f t="shared" si="15"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J198" s="1">
         <f t="shared" si="16"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K198" s="28"/>
       <c r="L198" s="2"/>
@@ -17788,11 +17794,11 @@
       </c>
       <c r="I199" s="1">
         <f t="shared" ref="I199:I262" si="21">J198</f>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J199" s="1">
         <f t="shared" ref="J199:J262" si="22">IF(K199="DONE",I199+(L199/1440)+(M199/86400),I199)</f>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K199" s="28"/>
       <c r="L199" s="2"/>
@@ -17834,11 +17840,11 @@
       </c>
       <c r="I200" s="1">
         <f t="shared" si="21"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J200" s="1">
         <f t="shared" si="22"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K200" s="28"/>
       <c r="L200" s="2"/>
@@ -17880,11 +17886,11 @@
       </c>
       <c r="I201" s="1">
         <f t="shared" si="21"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J201" s="1">
         <f t="shared" si="22"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K201" s="28"/>
       <c r="L201" s="2"/>
@@ -17926,11 +17932,11 @@
       </c>
       <c r="I202" s="1">
         <f t="shared" si="21"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J202" s="1">
         <f t="shared" si="22"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K202" s="28"/>
       <c r="L202" s="2"/>
@@ -17972,11 +17978,11 @@
       </c>
       <c r="I203" s="1">
         <f t="shared" si="21"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J203" s="1">
         <f t="shared" si="22"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K203" s="28"/>
       <c r="L203" s="2"/>
@@ -18018,11 +18024,11 @@
       </c>
       <c r="I204" s="1">
         <f t="shared" si="21"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J204" s="1">
         <f t="shared" si="22"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K204" s="28"/>
       <c r="L204" s="2"/>
@@ -18064,11 +18070,11 @@
       </c>
       <c r="I205" s="1">
         <f t="shared" si="21"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J205" s="1">
         <f t="shared" si="22"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K205" s="28"/>
       <c r="L205" s="2"/>
@@ -18110,11 +18116,11 @@
       </c>
       <c r="I206" s="1">
         <f t="shared" si="21"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J206" s="1">
         <f t="shared" si="22"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K206" s="28"/>
       <c r="L206" s="2"/>
@@ -18156,11 +18162,11 @@
       </c>
       <c r="I207" s="1">
         <f t="shared" si="21"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J207" s="1">
         <f t="shared" si="22"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K207" s="28"/>
       <c r="L207" s="2"/>
@@ -18202,11 +18208,11 @@
       </c>
       <c r="I208" s="1">
         <f t="shared" si="21"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J208" s="1">
         <f t="shared" si="22"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K208" s="28"/>
       <c r="L208" s="2"/>
@@ -18248,11 +18254,11 @@
       </c>
       <c r="I209" s="1">
         <f t="shared" si="21"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J209" s="1">
         <f t="shared" si="22"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K209" s="28"/>
       <c r="L209" s="2"/>
@@ -18294,11 +18300,11 @@
       </c>
       <c r="I210" s="1">
         <f t="shared" si="21"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J210" s="1">
         <f t="shared" si="22"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K210" s="28"/>
       <c r="L210" s="2"/>
@@ -18340,11 +18346,11 @@
       </c>
       <c r="I211" s="1">
         <f t="shared" si="21"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J211" s="1">
         <f t="shared" si="22"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K211" s="28"/>
       <c r="L211" s="2"/>
@@ -18386,11 +18392,11 @@
       </c>
       <c r="I212" s="1">
         <f t="shared" si="21"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J212" s="1">
         <f t="shared" si="22"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K212" s="28"/>
       <c r="L212" s="2"/>
@@ -18432,11 +18438,11 @@
       </c>
       <c r="I213" s="1">
         <f t="shared" si="21"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J213" s="1">
         <f t="shared" si="22"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K213" s="28"/>
       <c r="L213" s="2"/>
@@ -18478,11 +18484,11 @@
       </c>
       <c r="I214" s="1">
         <f t="shared" si="21"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J214" s="1">
         <f t="shared" si="22"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K214" s="28"/>
       <c r="L214" s="2"/>
@@ -18524,11 +18530,11 @@
       </c>
       <c r="I215" s="1">
         <f t="shared" si="21"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J215" s="1">
         <f t="shared" si="22"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K215" s="28"/>
       <c r="L215" s="2"/>
@@ -18570,11 +18576,11 @@
       </c>
       <c r="I216" s="1">
         <f t="shared" si="21"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J216" s="1">
         <f t="shared" si="22"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K216" s="28"/>
       <c r="L216" s="2"/>
@@ -18616,11 +18622,11 @@
       </c>
       <c r="I217" s="1">
         <f t="shared" si="21"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J217" s="1">
         <f t="shared" si="22"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K217" s="28"/>
       <c r="L217" s="2"/>
@@ -18662,11 +18668,11 @@
       </c>
       <c r="I218" s="1">
         <f t="shared" si="21"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J218" s="1">
         <f t="shared" si="22"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K218" s="28"/>
       <c r="L218" s="2"/>
@@ -18708,11 +18714,11 @@
       </c>
       <c r="I219" s="1">
         <f t="shared" si="21"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J219" s="1">
         <f t="shared" si="22"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K219" s="28"/>
       <c r="L219" s="2"/>
@@ -18754,11 +18760,11 @@
       </c>
       <c r="I220" s="1">
         <f t="shared" si="21"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J220" s="1">
         <f t="shared" si="22"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K220" s="28"/>
       <c r="L220" s="2"/>
@@ -18800,11 +18806,11 @@
       </c>
       <c r="I221" s="1">
         <f t="shared" si="21"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J221" s="1">
         <f t="shared" si="22"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K221" s="28"/>
       <c r="L221" s="2"/>
@@ -18846,11 +18852,11 @@
       </c>
       <c r="I222" s="1">
         <f t="shared" si="21"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J222" s="1">
         <f t="shared" si="22"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K222" s="28"/>
       <c r="L222" s="2"/>
@@ -18892,11 +18898,11 @@
       </c>
       <c r="I223" s="1">
         <f t="shared" si="21"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J223" s="1">
         <f t="shared" si="22"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K223" s="28"/>
       <c r="L223" s="2"/>
@@ -18938,11 +18944,11 @@
       </c>
       <c r="I224" s="1">
         <f t="shared" si="21"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J224" s="1">
         <f t="shared" si="22"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K224" s="28"/>
       <c r="L224" s="2"/>
@@ -18984,11 +18990,11 @@
       </c>
       <c r="I225" s="1">
         <f t="shared" si="21"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J225" s="1">
         <f t="shared" si="22"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K225" s="28"/>
       <c r="L225" s="2"/>
@@ -19030,11 +19036,11 @@
       </c>
       <c r="I226" s="1">
         <f t="shared" si="21"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J226" s="1">
         <f t="shared" si="22"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K226" s="28"/>
       <c r="L226" s="2"/>
@@ -19076,11 +19082,11 @@
       </c>
       <c r="I227" s="1">
         <f t="shared" si="21"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J227" s="1">
         <f t="shared" si="22"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K227" s="28"/>
       <c r="L227" s="2"/>
@@ -19122,11 +19128,11 @@
       </c>
       <c r="I228" s="1">
         <f t="shared" si="21"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J228" s="1">
         <f t="shared" si="22"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K228" s="28"/>
       <c r="L228" s="2"/>
@@ -19168,11 +19174,11 @@
       </c>
       <c r="I229" s="1">
         <f t="shared" si="21"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J229" s="1">
         <f t="shared" si="22"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K229" s="28"/>
       <c r="L229" s="2"/>
@@ -19214,11 +19220,11 @@
       </c>
       <c r="I230" s="1">
         <f t="shared" si="21"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J230" s="1">
         <f t="shared" si="22"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K230" s="28"/>
       <c r="L230" s="2"/>
@@ -19260,11 +19266,11 @@
       </c>
       <c r="I231" s="1">
         <f t="shared" si="21"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J231" s="1">
         <f t="shared" si="22"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K231" s="28"/>
       <c r="L231" s="2"/>
@@ -19306,11 +19312,11 @@
       </c>
       <c r="I232" s="1">
         <f t="shared" si="21"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J232" s="1">
         <f t="shared" si="22"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K232" s="28"/>
       <c r="L232" s="2"/>
@@ -19352,11 +19358,11 @@
       </c>
       <c r="I233" s="1">
         <f t="shared" si="21"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J233" s="1">
         <f t="shared" si="22"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K233" s="28"/>
       <c r="L233" s="2"/>
@@ -19398,11 +19404,11 @@
       </c>
       <c r="I234" s="1">
         <f t="shared" si="21"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J234" s="1">
         <f t="shared" si="22"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K234" s="28"/>
       <c r="L234" s="2"/>
@@ -19444,11 +19450,11 @@
       </c>
       <c r="I235" s="1">
         <f t="shared" si="21"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J235" s="1">
         <f t="shared" si="22"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K235" s="28"/>
       <c r="L235" s="2"/>
@@ -19490,11 +19496,11 @@
       </c>
       <c r="I236" s="1">
         <f t="shared" si="21"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J236" s="1">
         <f t="shared" si="22"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K236" s="28"/>
       <c r="L236" s="2"/>
@@ -19536,11 +19542,11 @@
       </c>
       <c r="I237" s="1">
         <f t="shared" si="21"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J237" s="1">
         <f t="shared" si="22"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K237" s="28"/>
       <c r="L237" s="2"/>
@@ -19582,11 +19588,11 @@
       </c>
       <c r="I238" s="1">
         <f t="shared" si="21"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J238" s="1">
         <f t="shared" si="22"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K238" s="28"/>
       <c r="L238" s="2"/>
@@ -19628,11 +19634,11 @@
       </c>
       <c r="I239" s="1">
         <f t="shared" si="21"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J239" s="1">
         <f t="shared" si="22"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K239" s="28"/>
       <c r="L239" s="2"/>
@@ -19674,11 +19680,11 @@
       </c>
       <c r="I240" s="1">
         <f t="shared" si="21"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J240" s="1">
         <f t="shared" si="22"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K240" s="28"/>
       <c r="L240" s="2"/>
@@ -19720,11 +19726,11 @@
       </c>
       <c r="I241" s="1">
         <f t="shared" si="21"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J241" s="1">
         <f t="shared" si="22"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K241" s="28"/>
       <c r="L241" s="2"/>
@@ -19766,11 +19772,11 @@
       </c>
       <c r="I242" s="1">
         <f t="shared" si="21"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J242" s="1">
         <f t="shared" si="22"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K242" s="28"/>
       <c r="L242" s="2"/>
@@ -19812,11 +19818,11 @@
       </c>
       <c r="I243" s="1">
         <f t="shared" si="21"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J243" s="1">
         <f t="shared" si="22"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K243" s="28"/>
       <c r="L243" s="2"/>
@@ -19858,11 +19864,11 @@
       </c>
       <c r="I244" s="1">
         <f t="shared" si="21"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J244" s="1">
         <f t="shared" si="22"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K244" s="28"/>
       <c r="L244" s="2"/>
@@ -19904,11 +19910,11 @@
       </c>
       <c r="I245" s="1">
         <f t="shared" si="21"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J245" s="1">
         <f t="shared" si="22"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K245" s="28"/>
       <c r="L245" s="2"/>
@@ -19950,11 +19956,11 @@
       </c>
       <c r="I246" s="1">
         <f t="shared" si="21"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J246" s="1">
         <f t="shared" si="22"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K246" s="28"/>
       <c r="L246" s="2"/>
@@ -19996,11 +20002,11 @@
       </c>
       <c r="I247" s="1">
         <f t="shared" si="21"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J247" s="1">
         <f t="shared" si="22"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K247" s="28"/>
       <c r="L247" s="2"/>
@@ -20042,11 +20048,11 @@
       </c>
       <c r="I248" s="1">
         <f t="shared" si="21"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J248" s="1">
         <f t="shared" si="22"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K248" s="28"/>
       <c r="L248" s="2"/>
@@ -20088,11 +20094,11 @@
       </c>
       <c r="I249" s="1">
         <f t="shared" si="21"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J249" s="1">
         <f t="shared" si="22"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K249" s="28"/>
       <c r="L249" s="2"/>
@@ -20134,11 +20140,11 @@
       </c>
       <c r="I250" s="1">
         <f t="shared" si="21"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J250" s="1">
         <f t="shared" si="22"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K250" s="28"/>
       <c r="L250" s="2"/>
@@ -20180,11 +20186,11 @@
       </c>
       <c r="I251" s="1">
         <f t="shared" si="21"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J251" s="1">
         <f t="shared" si="22"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K251" s="28"/>
       <c r="L251" s="2"/>
@@ -20226,11 +20232,11 @@
       </c>
       <c r="I252" s="1">
         <f t="shared" si="21"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J252" s="1">
         <f t="shared" si="22"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K252" s="28"/>
       <c r="L252" s="2"/>
@@ -20272,11 +20278,11 @@
       </c>
       <c r="I253" s="1">
         <f t="shared" si="21"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J253" s="1">
         <f t="shared" si="22"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K253" s="28"/>
       <c r="L253" s="2"/>
@@ -20318,11 +20324,11 @@
       </c>
       <c r="I254" s="1">
         <f t="shared" si="21"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J254" s="1">
         <f t="shared" si="22"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K254" s="28"/>
       <c r="L254" s="2"/>
@@ -20364,11 +20370,11 @@
       </c>
       <c r="I255" s="1">
         <f t="shared" si="21"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J255" s="1">
         <f t="shared" si="22"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K255" s="28"/>
       <c r="L255" s="2"/>
@@ -20410,11 +20416,11 @@
       </c>
       <c r="I256" s="1">
         <f t="shared" si="21"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J256" s="1">
         <f t="shared" si="22"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K256" s="28"/>
       <c r="L256" s="2"/>
@@ -20456,11 +20462,11 @@
       </c>
       <c r="I257" s="1">
         <f t="shared" si="21"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J257" s="1">
         <f t="shared" si="22"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K257" s="28"/>
       <c r="L257" s="2"/>
@@ -20502,11 +20508,11 @@
       </c>
       <c r="I258" s="1">
         <f t="shared" si="21"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J258" s="1">
         <f t="shared" si="22"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K258" s="28"/>
       <c r="L258" s="2"/>
@@ -20548,11 +20554,11 @@
       </c>
       <c r="I259" s="1">
         <f t="shared" si="21"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J259" s="1">
         <f t="shared" si="22"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K259" s="28"/>
       <c r="L259" s="2"/>
@@ -20594,11 +20600,11 @@
       </c>
       <c r="I260" s="1">
         <f t="shared" si="21"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J260" s="1">
         <f t="shared" si="22"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K260" s="28"/>
       <c r="L260" s="2"/>
@@ -20640,11 +20646,11 @@
       </c>
       <c r="I261" s="1">
         <f t="shared" si="21"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J261" s="1">
         <f t="shared" si="22"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K261" s="28"/>
       <c r="L261" s="2"/>
@@ -20686,11 +20692,11 @@
       </c>
       <c r="I262" s="1">
         <f t="shared" si="21"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J262" s="1">
         <f t="shared" si="22"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K262" s="28"/>
       <c r="L262" s="2"/>
@@ -20732,11 +20738,11 @@
       </c>
       <c r="I263" s="1">
         <f t="shared" ref="I263:I326" si="27">J262</f>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J263" s="1">
         <f t="shared" ref="J263:J326" si="28">IF(K263="DONE",I263+(L263/1440)+(M263/86400),I263)</f>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K263" s="28"/>
       <c r="L263" s="2"/>
@@ -20778,11 +20784,11 @@
       </c>
       <c r="I264" s="1">
         <f t="shared" si="27"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J264" s="1">
         <f t="shared" si="28"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K264" s="28"/>
       <c r="L264" s="2"/>
@@ -20824,11 +20830,11 @@
       </c>
       <c r="I265" s="1">
         <f t="shared" si="27"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J265" s="1">
         <f t="shared" si="28"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K265" s="28"/>
       <c r="L265" s="2"/>
@@ -20870,11 +20876,11 @@
       </c>
       <c r="I266" s="1">
         <f t="shared" si="27"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J266" s="1">
         <f t="shared" si="28"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K266" s="28"/>
       <c r="L266" s="2"/>
@@ -20916,11 +20922,11 @@
       </c>
       <c r="I267" s="1">
         <f t="shared" si="27"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J267" s="1">
         <f t="shared" si="28"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K267" s="28"/>
       <c r="L267" s="2"/>
@@ -20962,11 +20968,11 @@
       </c>
       <c r="I268" s="1">
         <f t="shared" si="27"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J268" s="1">
         <f t="shared" si="28"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K268" s="28"/>
       <c r="L268" s="2"/>
@@ -21008,11 +21014,11 @@
       </c>
       <c r="I269" s="1">
         <f t="shared" si="27"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J269" s="1">
         <f t="shared" si="28"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K269" s="28"/>
       <c r="L269" s="2"/>
@@ -21054,11 +21060,11 @@
       </c>
       <c r="I270" s="1">
         <f t="shared" si="27"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J270" s="1">
         <f t="shared" si="28"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K270" s="28"/>
       <c r="L270" s="2"/>
@@ -21100,11 +21106,11 @@
       </c>
       <c r="I271" s="1">
         <f t="shared" si="27"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J271" s="1">
         <f t="shared" si="28"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K271" s="28"/>
       <c r="L271" s="2"/>
@@ -21146,11 +21152,11 @@
       </c>
       <c r="I272" s="1">
         <f t="shared" si="27"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J272" s="1">
         <f t="shared" si="28"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K272" s="28"/>
       <c r="L272" s="2"/>
@@ -21192,11 +21198,11 @@
       </c>
       <c r="I273" s="1">
         <f t="shared" si="27"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J273" s="1">
         <f t="shared" si="28"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K273" s="28"/>
       <c r="L273" s="2"/>
@@ -21238,11 +21244,11 @@
       </c>
       <c r="I274" s="1">
         <f t="shared" si="27"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J274" s="1">
         <f t="shared" si="28"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K274" s="28"/>
       <c r="L274" s="2"/>
@@ -21284,11 +21290,11 @@
       </c>
       <c r="I275" s="1">
         <f t="shared" si="27"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J275" s="1">
         <f t="shared" si="28"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K275" s="28"/>
       <c r="L275" s="2"/>
@@ -21330,11 +21336,11 @@
       </c>
       <c r="I276" s="1">
         <f t="shared" si="27"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J276" s="1">
         <f t="shared" si="28"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K276" s="28"/>
       <c r="L276" s="2"/>
@@ -21376,11 +21382,11 @@
       </c>
       <c r="I277" s="1">
         <f t="shared" si="27"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J277" s="1">
         <f t="shared" si="28"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K277" s="28"/>
       <c r="L277" s="2"/>
@@ -21422,11 +21428,11 @@
       </c>
       <c r="I278" s="1">
         <f t="shared" si="27"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J278" s="1">
         <f t="shared" si="28"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K278" s="28"/>
       <c r="L278" s="2"/>
@@ -21468,11 +21474,11 @@
       </c>
       <c r="I279" s="1">
         <f t="shared" si="27"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J279" s="1">
         <f t="shared" si="28"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K279" s="28"/>
       <c r="L279" s="2"/>
@@ -21514,11 +21520,11 @@
       </c>
       <c r="I280" s="1">
         <f t="shared" si="27"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J280" s="1">
         <f t="shared" si="28"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K280" s="28"/>
       <c r="L280" s="2"/>
@@ -21560,11 +21566,11 @@
       </c>
       <c r="I281" s="1">
         <f t="shared" si="27"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J281" s="1">
         <f t="shared" si="28"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K281" s="28"/>
       <c r="L281" s="2"/>
@@ -21606,11 +21612,11 @@
       </c>
       <c r="I282" s="1">
         <f t="shared" si="27"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J282" s="1">
         <f t="shared" si="28"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K282" s="28"/>
       <c r="L282" s="2"/>
@@ -21652,11 +21658,11 @@
       </c>
       <c r="I283" s="1">
         <f t="shared" si="27"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J283" s="1">
         <f t="shared" si="28"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K283" s="28"/>
       <c r="L283" s="2"/>
@@ -21698,11 +21704,11 @@
       </c>
       <c r="I284" s="1">
         <f t="shared" si="27"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J284" s="1">
         <f t="shared" si="28"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K284" s="28"/>
       <c r="L284" s="2"/>
@@ -21744,11 +21750,11 @@
       </c>
       <c r="I285" s="1">
         <f t="shared" si="27"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J285" s="1">
         <f t="shared" si="28"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K285" s="28"/>
       <c r="L285" s="2"/>
@@ -21790,11 +21796,11 @@
       </c>
       <c r="I286" s="1">
         <f t="shared" si="27"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J286" s="1">
         <f t="shared" si="28"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K286" s="28"/>
       <c r="L286" s="2"/>
@@ -21836,11 +21842,11 @@
       </c>
       <c r="I287" s="1">
         <f t="shared" si="27"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J287" s="1">
         <f t="shared" si="28"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K287" s="28"/>
       <c r="L287" s="2"/>
@@ -21882,11 +21888,11 @@
       </c>
       <c r="I288" s="1">
         <f t="shared" si="27"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J288" s="1">
         <f t="shared" si="28"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K288" s="28"/>
       <c r="L288" s="2"/>
@@ -21928,11 +21934,11 @@
       </c>
       <c r="I289" s="1">
         <f t="shared" si="27"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J289" s="1">
         <f t="shared" si="28"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K289" s="28"/>
       <c r="L289" s="2"/>
@@ -21974,11 +21980,11 @@
       </c>
       <c r="I290" s="1">
         <f t="shared" si="27"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J290" s="1">
         <f t="shared" si="28"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K290" s="28"/>
       <c r="L290" s="2"/>
@@ -22020,11 +22026,11 @@
       </c>
       <c r="I291" s="1">
         <f t="shared" si="27"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J291" s="1">
         <f t="shared" si="28"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K291" s="28"/>
       <c r="L291" s="2"/>
@@ -22066,11 +22072,11 @@
       </c>
       <c r="I292" s="1">
         <f t="shared" si="27"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J292" s="1">
         <f t="shared" si="28"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K292" s="28"/>
       <c r="L292" s="2"/>
@@ -22112,11 +22118,11 @@
       </c>
       <c r="I293" s="1">
         <f t="shared" si="27"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J293" s="1">
         <f t="shared" si="28"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K293" s="28"/>
       <c r="L293" s="2"/>
@@ -22158,11 +22164,11 @@
       </c>
       <c r="I294" s="1">
         <f t="shared" si="27"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J294" s="1">
         <f t="shared" si="28"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K294" s="28"/>
       <c r="L294" s="2"/>
@@ -22204,11 +22210,11 @@
       </c>
       <c r="I295" s="1">
         <f t="shared" si="27"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J295" s="1">
         <f t="shared" si="28"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K295" s="28"/>
       <c r="L295" s="2"/>
@@ -22250,11 +22256,11 @@
       </c>
       <c r="I296" s="1">
         <f t="shared" si="27"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J296" s="1">
         <f t="shared" si="28"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K296" s="28"/>
       <c r="L296" s="2"/>
@@ -22296,11 +22302,11 @@
       </c>
       <c r="I297" s="1">
         <f t="shared" si="27"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J297" s="1">
         <f t="shared" si="28"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K297" s="28"/>
       <c r="L297" s="2"/>
@@ -22342,11 +22348,11 @@
       </c>
       <c r="I298" s="1">
         <f t="shared" si="27"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J298" s="1">
         <f t="shared" si="28"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K298" s="28"/>
       <c r="L298" s="2"/>
@@ -22388,11 +22394,11 @@
       </c>
       <c r="I299" s="1">
         <f t="shared" si="27"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J299" s="1">
         <f t="shared" si="28"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K299" s="28"/>
       <c r="L299" s="2"/>
@@ -22434,11 +22440,11 @@
       </c>
       <c r="I300" s="1">
         <f t="shared" si="27"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J300" s="1">
         <f t="shared" si="28"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K300" s="28"/>
       <c r="L300" s="2"/>
@@ -22480,11 +22486,11 @@
       </c>
       <c r="I301" s="1">
         <f t="shared" si="27"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J301" s="1">
         <f t="shared" si="28"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K301" s="28"/>
       <c r="L301" s="2"/>
@@ -22526,11 +22532,11 @@
       </c>
       <c r="I302" s="1">
         <f t="shared" si="27"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J302" s="1">
         <f t="shared" si="28"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K302" s="28"/>
       <c r="L302" s="2"/>
@@ -22572,11 +22578,11 @@
       </c>
       <c r="I303" s="1">
         <f t="shared" si="27"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J303" s="1">
         <f t="shared" si="28"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K303" s="28"/>
       <c r="L303" s="2"/>
@@ -22618,11 +22624,11 @@
       </c>
       <c r="I304" s="1">
         <f t="shared" si="27"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J304" s="1">
         <f t="shared" si="28"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K304" s="28"/>
       <c r="L304" s="2"/>
@@ -22664,11 +22670,11 @@
       </c>
       <c r="I305" s="1">
         <f t="shared" si="27"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J305" s="1">
         <f t="shared" si="28"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K305" s="28"/>
       <c r="L305" s="2"/>
@@ -22710,11 +22716,11 @@
       </c>
       <c r="I306" s="1">
         <f t="shared" si="27"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J306" s="1">
         <f t="shared" si="28"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K306" s="28"/>
       <c r="L306" s="2"/>
@@ -22756,11 +22762,11 @@
       </c>
       <c r="I307" s="1">
         <f t="shared" si="27"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J307" s="1">
         <f t="shared" si="28"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K307" s="28"/>
       <c r="L307" s="2"/>
@@ -22802,11 +22808,11 @@
       </c>
       <c r="I308" s="1">
         <f t="shared" si="27"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J308" s="1">
         <f t="shared" si="28"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K308" s="28"/>
       <c r="L308" s="2"/>
@@ -22848,11 +22854,11 @@
       </c>
       <c r="I309" s="1">
         <f t="shared" si="27"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J309" s="1">
         <f t="shared" si="28"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K309" s="28"/>
       <c r="L309" s="2"/>
@@ -22894,11 +22900,11 @@
       </c>
       <c r="I310" s="1">
         <f t="shared" si="27"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J310" s="1">
         <f t="shared" si="28"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K310" s="28"/>
       <c r="L310" s="2"/>
@@ -22940,11 +22946,11 @@
       </c>
       <c r="I311" s="1">
         <f t="shared" si="27"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J311" s="1">
         <f t="shared" si="28"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K311" s="28"/>
       <c r="L311" s="2"/>
@@ -22986,11 +22992,11 @@
       </c>
       <c r="I312" s="1">
         <f t="shared" si="27"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J312" s="1">
         <f t="shared" si="28"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K312" s="28"/>
       <c r="L312" s="2"/>
@@ -23032,11 +23038,11 @@
       </c>
       <c r="I313" s="1">
         <f t="shared" si="27"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J313" s="1">
         <f t="shared" si="28"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K313" s="28"/>
       <c r="L313" s="2"/>
@@ -23078,11 +23084,11 @@
       </c>
       <c r="I314" s="1">
         <f t="shared" si="27"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J314" s="1">
         <f t="shared" si="28"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K314" s="28"/>
       <c r="L314" s="2"/>
@@ -23124,11 +23130,11 @@
       </c>
       <c r="I315" s="1">
         <f t="shared" si="27"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J315" s="1">
         <f t="shared" si="28"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K315" s="28"/>
       <c r="L315" s="2"/>
@@ -23170,11 +23176,11 @@
       </c>
       <c r="I316" s="1">
         <f t="shared" si="27"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J316" s="1">
         <f t="shared" si="28"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K316" s="28"/>
       <c r="L316" s="2"/>
@@ -23216,11 +23222,11 @@
       </c>
       <c r="I317" s="1">
         <f t="shared" si="27"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J317" s="1">
         <f t="shared" si="28"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K317" s="28"/>
       <c r="L317" s="2"/>
@@ -23262,11 +23268,11 @@
       </c>
       <c r="I318" s="1">
         <f t="shared" si="27"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J318" s="1">
         <f t="shared" si="28"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K318" s="28"/>
       <c r="L318" s="2"/>
@@ -23308,11 +23314,11 @@
       </c>
       <c r="I319" s="1">
         <f t="shared" si="27"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J319" s="1">
         <f t="shared" si="28"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K319" s="28"/>
       <c r="L319" s="2"/>
@@ -23354,11 +23360,11 @@
       </c>
       <c r="I320" s="1">
         <f t="shared" si="27"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J320" s="1">
         <f t="shared" si="28"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K320" s="28"/>
       <c r="L320" s="2"/>
@@ -23400,11 +23406,11 @@
       </c>
       <c r="I321" s="1">
         <f t="shared" si="27"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J321" s="1">
         <f t="shared" si="28"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K321" s="28"/>
       <c r="L321" s="2"/>
@@ -23446,11 +23452,11 @@
       </c>
       <c r="I322" s="1">
         <f t="shared" si="27"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J322" s="1">
         <f t="shared" si="28"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K322" s="28"/>
       <c r="L322" s="2"/>
@@ -23492,11 +23498,11 @@
       </c>
       <c r="I323" s="1">
         <f t="shared" si="27"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J323" s="1">
         <f t="shared" si="28"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K323" s="28"/>
       <c r="L323" s="2"/>
@@ -23538,11 +23544,11 @@
       </c>
       <c r="I324" s="1">
         <f t="shared" si="27"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J324" s="1">
         <f t="shared" si="28"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K324" s="28"/>
       <c r="L324" s="2"/>
@@ -23584,11 +23590,11 @@
       </c>
       <c r="I325" s="1">
         <f t="shared" si="27"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J325" s="1">
         <f t="shared" si="28"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K325" s="28"/>
       <c r="L325" s="2"/>
@@ -23630,11 +23636,11 @@
       </c>
       <c r="I326" s="1">
         <f t="shared" si="27"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J326" s="1">
         <f t="shared" si="28"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K326" s="28"/>
       <c r="L326" s="2"/>
@@ -23676,11 +23682,11 @@
       </c>
       <c r="I327" s="1">
         <f t="shared" ref="I327:I369" si="33">J326</f>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J327" s="1">
         <f t="shared" ref="J327:J369" si="34">IF(K327="DONE",I327+(L327/1440)+(M327/86400),I327)</f>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K327" s="28"/>
       <c r="L327" s="2"/>
@@ -23722,11 +23728,11 @@
       </c>
       <c r="I328" s="1">
         <f t="shared" si="33"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J328" s="1">
         <f t="shared" si="34"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K328" s="28"/>
       <c r="L328" s="2"/>
@@ -23768,11 +23774,11 @@
       </c>
       <c r="I329" s="1">
         <f t="shared" si="33"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J329" s="1">
         <f t="shared" si="34"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K329" s="28"/>
       <c r="L329" s="2"/>
@@ -23814,11 +23820,11 @@
       </c>
       <c r="I330" s="1">
         <f t="shared" si="33"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J330" s="1">
         <f t="shared" si="34"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K330" s="28"/>
       <c r="L330" s="2"/>
@@ -23860,11 +23866,11 @@
       </c>
       <c r="I331" s="1">
         <f t="shared" si="33"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J331" s="1">
         <f t="shared" si="34"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K331" s="28"/>
       <c r="L331" s="2"/>
@@ -23906,11 +23912,11 @@
       </c>
       <c r="I332" s="1">
         <f t="shared" si="33"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J332" s="1">
         <f t="shared" si="34"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K332" s="28"/>
       <c r="L332" s="2"/>
@@ -23952,11 +23958,11 @@
       </c>
       <c r="I333" s="1">
         <f t="shared" si="33"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J333" s="1">
         <f t="shared" si="34"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K333" s="28"/>
       <c r="L333" s="2"/>
@@ -23998,11 +24004,11 @@
       </c>
       <c r="I334" s="1">
         <f t="shared" si="33"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J334" s="1">
         <f t="shared" si="34"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K334" s="28"/>
       <c r="L334" s="2"/>
@@ -24044,11 +24050,11 @@
       </c>
       <c r="I335" s="1">
         <f t="shared" si="33"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J335" s="1">
         <f t="shared" si="34"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K335" s="28"/>
       <c r="L335" s="2"/>
@@ -24090,11 +24096,11 @@
       </c>
       <c r="I336" s="1">
         <f t="shared" si="33"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J336" s="1">
         <f t="shared" si="34"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K336" s="28"/>
       <c r="L336" s="2"/>
@@ -24136,11 +24142,11 @@
       </c>
       <c r="I337" s="1">
         <f t="shared" si="33"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J337" s="1">
         <f t="shared" si="34"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K337" s="28"/>
       <c r="L337" s="2"/>
@@ -24182,11 +24188,11 @@
       </c>
       <c r="I338" s="1">
         <f t="shared" si="33"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J338" s="1">
         <f t="shared" si="34"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K338" s="28"/>
       <c r="L338" s="2"/>
@@ -24228,11 +24234,11 @@
       </c>
       <c r="I339" s="1">
         <f t="shared" si="33"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J339" s="1">
         <f t="shared" si="34"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K339" s="28"/>
       <c r="L339" s="2"/>
@@ -24274,11 +24280,11 @@
       </c>
       <c r="I340" s="1">
         <f t="shared" si="33"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J340" s="1">
         <f t="shared" si="34"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K340" s="28"/>
       <c r="L340" s="2"/>
@@ -24320,11 +24326,11 @@
       </c>
       <c r="I341" s="1">
         <f t="shared" si="33"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J341" s="1">
         <f t="shared" si="34"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K341" s="28"/>
       <c r="L341" s="2"/>
@@ -24366,11 +24372,11 @@
       </c>
       <c r="I342" s="1">
         <f t="shared" si="33"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J342" s="1">
         <f t="shared" si="34"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K342" s="28"/>
       <c r="L342" s="2"/>
@@ -24412,11 +24418,11 @@
       </c>
       <c r="I343" s="1">
         <f t="shared" si="33"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J343" s="1">
         <f t="shared" si="34"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K343" s="28"/>
       <c r="L343" s="2"/>
@@ -24458,11 +24464,11 @@
       </c>
       <c r="I344" s="1">
         <f t="shared" si="33"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J344" s="1">
         <f t="shared" si="34"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K344" s="28"/>
       <c r="L344" s="2"/>
@@ -24504,11 +24510,11 @@
       </c>
       <c r="I345" s="1">
         <f t="shared" si="33"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J345" s="1">
         <f t="shared" si="34"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K345" s="28"/>
       <c r="L345" s="2"/>
@@ -24550,11 +24556,11 @@
       </c>
       <c r="I346" s="1">
         <f t="shared" si="33"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J346" s="1">
         <f t="shared" si="34"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K346" s="28"/>
       <c r="L346" s="2"/>
@@ -24596,11 +24602,11 @@
       </c>
       <c r="I347" s="1">
         <f t="shared" si="33"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J347" s="1">
         <f t="shared" si="34"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K347" s="28"/>
       <c r="L347" s="2"/>
@@ -24642,11 +24648,11 @@
       </c>
       <c r="I348" s="1">
         <f t="shared" si="33"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J348" s="1">
         <f t="shared" si="34"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K348" s="28"/>
       <c r="L348" s="2"/>
@@ -24688,11 +24694,11 @@
       </c>
       <c r="I349" s="1">
         <f t="shared" si="33"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J349" s="1">
         <f t="shared" si="34"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K349" s="28"/>
       <c r="L349" s="2"/>
@@ -24734,11 +24740,11 @@
       </c>
       <c r="I350" s="1">
         <f t="shared" si="33"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J350" s="1">
         <f t="shared" si="34"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K350" s="28"/>
       <c r="L350" s="2"/>
@@ -24780,11 +24786,11 @@
       </c>
       <c r="I351" s="1">
         <f t="shared" si="33"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J351" s="1">
         <f t="shared" si="34"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K351" s="28"/>
       <c r="L351" s="2"/>
@@ -24826,11 +24832,11 @@
       </c>
       <c r="I352" s="1">
         <f t="shared" si="33"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J352" s="1">
         <f t="shared" si="34"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K352" s="28"/>
       <c r="L352" s="2"/>
@@ -24872,11 +24878,11 @@
       </c>
       <c r="I353" s="1">
         <f t="shared" si="33"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J353" s="1">
         <f t="shared" si="34"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K353" s="28"/>
       <c r="L353" s="2"/>
@@ -24918,11 +24924,11 @@
       </c>
       <c r="I354" s="1">
         <f t="shared" si="33"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J354" s="1">
         <f t="shared" si="34"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K354" s="28"/>
       <c r="L354" s="2"/>
@@ -24964,11 +24970,11 @@
       </c>
       <c r="I355" s="1">
         <f t="shared" si="33"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J355" s="1">
         <f t="shared" si="34"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K355" s="28"/>
       <c r="L355" s="2"/>
@@ -25010,11 +25016,11 @@
       </c>
       <c r="I356" s="1">
         <f t="shared" si="33"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J356" s="1">
         <f t="shared" si="34"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K356" s="28"/>
       <c r="L356" s="2"/>
@@ -25056,11 +25062,11 @@
       </c>
       <c r="I357" s="1">
         <f t="shared" si="33"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J357" s="1">
         <f t="shared" si="34"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K357" s="28"/>
       <c r="L357" s="2"/>
@@ -25102,11 +25108,11 @@
       </c>
       <c r="I358" s="1">
         <f t="shared" si="33"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J358" s="1">
         <f t="shared" si="34"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K358" s="28"/>
       <c r="L358" s="2"/>
@@ -25148,11 +25154,11 @@
       </c>
       <c r="I359" s="1">
         <f t="shared" si="33"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J359" s="1">
         <f t="shared" si="34"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K359" s="28"/>
       <c r="L359" s="2"/>
@@ -25194,11 +25200,11 @@
       </c>
       <c r="I360" s="1">
         <f t="shared" si="33"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J360" s="1">
         <f t="shared" si="34"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K360" s="28"/>
       <c r="L360" s="2"/>
@@ -25240,11 +25246,11 @@
       </c>
       <c r="I361" s="1">
         <f t="shared" si="33"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J361" s="1">
         <f t="shared" si="34"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K361" s="28"/>
       <c r="L361" s="2"/>
@@ -25286,11 +25292,11 @@
       </c>
       <c r="I362" s="1">
         <f t="shared" si="33"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J362" s="1">
         <f t="shared" si="34"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K362" s="28"/>
       <c r="L362" s="2"/>
@@ -25332,11 +25338,11 @@
       </c>
       <c r="I363" s="1">
         <f t="shared" si="33"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J363" s="1">
         <f t="shared" si="34"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K363" s="28"/>
       <c r="L363" s="2"/>
@@ -25378,11 +25384,11 @@
       </c>
       <c r="I364" s="1">
         <f t="shared" si="33"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J364" s="1">
         <f t="shared" si="34"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K364" s="28"/>
       <c r="L364" s="2"/>
@@ -25424,11 +25430,11 @@
       </c>
       <c r="I365" s="1">
         <f t="shared" si="33"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J365" s="1">
         <f t="shared" si="34"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K365" s="28"/>
       <c r="L365" s="2"/>
@@ -25470,11 +25476,11 @@
       </c>
       <c r="I366" s="1">
         <f t="shared" si="33"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J366" s="1">
         <f t="shared" si="34"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K366" s="28"/>
       <c r="L366" s="2"/>
@@ -25516,11 +25522,11 @@
       </c>
       <c r="I367" s="1">
         <f t="shared" si="33"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J367" s="1">
         <f t="shared" si="34"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K367" s="28"/>
       <c r="L367" s="2"/>
@@ -25562,11 +25568,11 @@
       </c>
       <c r="I368" s="1">
         <f t="shared" si="33"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J368" s="1">
         <f t="shared" si="34"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K368" s="28"/>
       <c r="L368" s="2"/>
@@ -25608,11 +25614,11 @@
       </c>
       <c r="I369" s="1">
         <f t="shared" si="33"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="J369" s="1">
         <f t="shared" si="34"/>
-        <v>4.5937499999999985E-2</v>
+        <v>5.2094907407407388E-2</v>
       </c>
       <c r="K369" s="28"/>
       <c r="L369" s="2"/>
@@ -25741,22 +25747,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="106.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
     </row>
     <row r="2" spans="1:6" ht="25.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="47" t="s">
+      <c r="A2" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="47"/>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
       <c r="E2" s="3" t="s">
         <v>4</v>
       </c>
@@ -25765,10 +25771,10 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="25.2" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="47"/>
-      <c r="B3" s="47"/>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
+      <c r="A3" s="46"/>
+      <c r="B3" s="46"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
       <c r="E3" s="5">
         <f ca="1">(E4+(F4/60))/60</f>
         <v>8.3333333333333332E-3</v>
@@ -31731,22 +31737,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="106.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
     </row>
     <row r="2" spans="1:6" ht="25.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="55" t="s">
+      <c r="A2" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="55"/>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
+      <c r="B2" s="54"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
       <c r="E2" s="3" t="s">
         <v>4</v>
       </c>
@@ -31755,10 +31761,10 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="25.2" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="55"/>
-      <c r="B3" s="55"/>
-      <c r="C3" s="55"/>
-      <c r="D3" s="55"/>
+      <c r="A3" s="54"/>
+      <c r="B3" s="54"/>
+      <c r="C3" s="54"/>
+      <c r="D3" s="54"/>
       <c r="E3" s="5">
         <f ca="1">(E4+(F4/60))/60</f>
         <v>0.27500000000000002</v>
@@ -34501,22 +34507,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="106.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
     </row>
     <row r="2" spans="1:6" ht="25.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="56" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="56"/>
-      <c r="C2" s="56"/>
-      <c r="D2" s="56"/>
+      <c r="A2" s="55" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="55"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
       <c r="E2" s="3" t="s">
         <v>4</v>
       </c>
@@ -34525,10 +34531,10 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="25.2" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="56"/>
-      <c r="B3" s="56"/>
-      <c r="C3" s="56"/>
-      <c r="D3" s="56"/>
+      <c r="A3" s="55"/>
+      <c r="B3" s="55"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
       <c r="E3" s="5">
         <f ca="1">(E4+(F4/60))/60</f>
         <v>0.13333333333333333</v>
@@ -39996,22 +40002,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="106.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
     </row>
     <row r="2" spans="1:6" ht="25.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="57" t="s">
+      <c r="A2" s="56" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="57"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
+      <c r="B2" s="56"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
       <c r="E2" s="3" t="s">
         <v>4</v>
       </c>
@@ -40020,10 +40026,10 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="25.2" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="57"/>
-      <c r="B3" s="57"/>
-      <c r="C3" s="57"/>
-      <c r="D3" s="57"/>
+      <c r="A3" s="56"/>
+      <c r="B3" s="56"/>
+      <c r="C3" s="56"/>
+      <c r="D3" s="56"/>
       <c r="E3" s="5">
         <f ca="1">(E4+(F4/60))/60</f>
         <v>0.40555555555555561</v>
@@ -45797,22 +45803,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="106.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
     </row>
     <row r="2" spans="1:6" ht="25.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="57" t="s">
+      <c r="A2" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="57"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
+      <c r="B2" s="56"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
       <c r="E2" s="3" t="s">
         <v>4</v>
       </c>
@@ -45821,10 +45827,10 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="25.2" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="57"/>
-      <c r="B3" s="57"/>
-      <c r="C3" s="57"/>
-      <c r="D3" s="57"/>
+      <c r="A3" s="56"/>
+      <c r="B3" s="56"/>
+      <c r="C3" s="56"/>
+      <c r="D3" s="56"/>
       <c r="E3" s="5">
         <f ca="1">(E4+(F4/60))/60</f>
         <v>0</v>
@@ -51413,22 +51419,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="106.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
     </row>
     <row r="2" spans="1:7" ht="25.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="57" t="s">
+      <c r="A2" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="57"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
+      <c r="B2" s="56"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
       <c r="E2" s="3" t="s">
         <v>4</v>
       </c>
@@ -51437,10 +51443,10 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="25.2" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="57"/>
-      <c r="B3" s="57"/>
-      <c r="C3" s="57"/>
-      <c r="D3" s="57"/>
+      <c r="A3" s="56"/>
+      <c r="B3" s="56"/>
+      <c r="C3" s="56"/>
+      <c r="D3" s="56"/>
       <c r="E3" s="5">
         <f ca="1">(E4+(F4/60))/60</f>
         <v>0.33583333333333332</v>
@@ -57219,42 +57225,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="106.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="46" t="s">
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
-      <c r="K1" s="54"/>
-      <c r="L1" s="54"/>
+      <c r="H1" s="53"/>
+      <c r="I1" s="53"/>
+      <c r="J1" s="53"/>
+      <c r="K1" s="53"/>
+      <c r="L1" s="53"/>
     </row>
     <row r="2" spans="1:12" ht="25.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="57" t="s">
+      <c r="A2" s="56" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="57"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
+      <c r="B2" s="56"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
       <c r="E2" s="3" t="s">
         <v>4</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="57" t="s">
+      <c r="G2" s="56" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="57"/>
-      <c r="I2" s="57"/>
-      <c r="J2" s="57"/>
+      <c r="H2" s="56"/>
+      <c r="I2" s="56"/>
+      <c r="J2" s="56"/>
       <c r="K2" s="3" t="s">
         <v>4</v>
       </c>
@@ -57263,10 +57269,10 @@
       </c>
     </row>
     <row r="3" spans="1:12" ht="25.2" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="57"/>
-      <c r="B3" s="57"/>
-      <c r="C3" s="57"/>
-      <c r="D3" s="57"/>
+      <c r="A3" s="56"/>
+      <c r="B3" s="56"/>
+      <c r="C3" s="56"/>
+      <c r="D3" s="56"/>
       <c r="E3" s="5">
         <f ca="1">(E4+(F4/60))/60</f>
         <v>0.17277777777777778</v>
@@ -57275,10 +57281,10 @@
         <f ca="1">(E4+(F4/60))</f>
         <v>10.366666666666667</v>
       </c>
-      <c r="G3" s="57"/>
-      <c r="H3" s="57"/>
-      <c r="I3" s="57"/>
-      <c r="J3" s="57"/>
+      <c r="G3" s="56"/>
+      <c r="H3" s="56"/>
+      <c r="I3" s="56"/>
+      <c r="J3" s="56"/>
       <c r="K3" s="5">
         <f ca="1">(K4+(L4/60))/60</f>
         <v>1.3444444444444446</v>

</xml_diff>